<commit_message>
Needed to add tolerance to 16 block model.
</commit_message>
<xml_diff>
--- a/doc/multiples_of_3_95.xlsx
+++ b/doc/multiples_of_3_95.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\projects\block_bot\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\projects\blocks\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC90848-AC95-4573-B61B-E6478DB8D4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE694D9-1656-44E4-B4DF-E68E57027FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="1830" windowWidth="13065" windowHeight="12735" xr2:uid="{DE0F1C7F-B8E8-4D46-AC98-965DF7E088DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{DE0F1C7F-B8E8-4D46-AC98-965DF7E088DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,6 +98,9 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -115,9 +118,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -132,11 +132,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1087D735-E547-4B93-B662-3A1F6F374AF3}" name="Table1" displayName="Table1" ref="A2:B22" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1087D735-E547-4B93-B662-3A1F6F374AF3}" name="Table1" displayName="Table1" ref="A2:B22" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A2:B22" xr:uid="{1087D735-E547-4B93-B662-3A1F6F374AF3}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{CC53DC14-0684-4211-8D4D-1452626997A8}" name="N"/>
-    <tableColumn id="2" xr3:uid="{1983B5C3-53AE-4A86-A288-EEF15374214B}" name="Value" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{1983B5C3-53AE-4A86-A288-EEF15374214B}" name="Value" dataDxfId="0">
       <calculatedColumnFormula>A3*3.95</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -444,7 +444,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>